<commit_message>
Pivot tables, arrays, sequences
</commit_message>
<xml_diff>
--- a/advanced_tutorial.xlsx
+++ b/advanced_tutorial.xlsx
@@ -8,24 +8,46 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mymac/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DA78C4-5724-6145-AA36-D14DEA2D7543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36D3097-E7A0-1E4E-92A8-115EFA3C1671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{9E1E0ABE-1EFE-9045-A75B-5CB98AFF96A8}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{9E1E0ABE-1EFE-9045-A75B-5CB98AFF96A8}"/>
   </bookViews>
   <sheets>
     <sheet name="namedRanges" sheetId="1" r:id="rId1"/>
     <sheet name="vLookup" sheetId="2" r:id="rId2"/>
     <sheet name="pivotTables" sheetId="3" r:id="rId3"/>
+    <sheet name="arrays" sheetId="4" r:id="rId4"/>
+    <sheet name="sequence" sheetId="5" r:id="rId5"/>
+    <sheet name="xLookup" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Customer">namedRanges!$B$2:$B$15</definedName>
+    <definedName name="Month">pivotTables!$A$2:$A$14</definedName>
     <definedName name="Order">namedRanges!$A$2:$A$15</definedName>
     <definedName name="Price_Per_Unit">namedRanges!$D$2:$D$15</definedName>
     <definedName name="Quantity">namedRanges!$C$2:$C$15</definedName>
+    <definedName name="Slicer_Category">#N/A</definedName>
+    <definedName name="Slicer_Manager">#N/A</definedName>
+    <definedName name="Slicer_Store">#N/A</definedName>
+    <definedName name="Slicer_Town">#N/A</definedName>
     <definedName name="Total">namedRanges!$E$2:$E$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="0" r:id="rId7"/>
+  </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId8"/>
+        <x14:slicerCache r:id="rId9"/>
+        <x14:slicerCache r:id="rId10"/>
+        <x14:slicerCache r:id="rId11"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -44,8 +66,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="111">
   <si>
     <t>Order #</t>
   </si>
@@ -159,18 +203,238 @@
   </si>
   <si>
     <t>Part 9</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>Town</t>
+  </si>
+  <si>
+    <t>Store Code</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Computech</t>
+  </si>
+  <si>
+    <t>MicroWorld</t>
+  </si>
+  <si>
+    <t>Aberdeen</t>
+  </si>
+  <si>
+    <t>ABD</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Jason Hervey</t>
+  </si>
+  <si>
+    <t>Spencer Lee</t>
+  </si>
+  <si>
+    <t>Hugo Matthews</t>
+  </si>
+  <si>
+    <t>Ben Malone</t>
+  </si>
+  <si>
+    <t>Kirsty Young</t>
+  </si>
+  <si>
+    <t>Jade Wilson</t>
+  </si>
+  <si>
+    <t>Craig Spinks</t>
+  </si>
+  <si>
+    <t>Nick Fallows</t>
+  </si>
+  <si>
+    <t>Stephanie Zanoni</t>
+  </si>
+  <si>
+    <t>Sam Waters</t>
+  </si>
+  <si>
+    <t>Frank Archibald</t>
+  </si>
+  <si>
+    <t>Mobile Phones</t>
+  </si>
+  <si>
+    <t>PC's</t>
+  </si>
+  <si>
+    <t>Laptops</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>Printers</t>
+  </si>
+  <si>
+    <t>Cameras</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Sales</t>
+  </si>
+  <si>
+    <t>Average of Sales</t>
+  </si>
+  <si>
+    <t>Spencer Lee Total</t>
+  </si>
+  <si>
+    <t>Craig Spinks Total</t>
+  </si>
+  <si>
+    <t>Hugo Matthews Total</t>
+  </si>
+  <si>
+    <t>Jason Hervey Total</t>
+  </si>
+  <si>
+    <t>Nick Fallows Total</t>
+  </si>
+  <si>
+    <t>Sam Waters Total</t>
+  </si>
+  <si>
+    <t>Kirsty Young Total</t>
+  </si>
+  <si>
+    <t>Ben Malone Total</t>
+  </si>
+  <si>
+    <t>Jade Wilson Total</t>
+  </si>
+  <si>
+    <t>Stephanie Zanoni Total</t>
+  </si>
+  <si>
+    <t>Frank Archibald Total</t>
+  </si>
+  <si>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Price per Item</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Grapes</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Random array</t>
+  </si>
+  <si>
+    <t>Sort (by price per item, descending)</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Social Media</t>
+  </si>
+  <si>
+    <t>Temple Run</t>
+  </si>
+  <si>
+    <t>Candy Crush</t>
+  </si>
+  <si>
+    <t>Doom</t>
+  </si>
+  <si>
+    <t>Bejewelled</t>
+  </si>
+  <si>
+    <t>Office Lens</t>
+  </si>
+  <si>
+    <t>Google Docs</t>
+  </si>
+  <si>
+    <t>OneDrive</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>In-App Purchases</t>
+  </si>
+  <si>
+    <t>Free</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -204,6 +468,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -213,12 +484,21 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -227,13 +507,25 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -243,7 +535,81 @@
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -254,6 +620,867 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>333130</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>2932</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>42007</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>160457</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Store">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72F7A456-5899-3C98-A432-CF13B38C6A3F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Store"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3869592" y="3490547"/>
+              <a:ext cx="1828800" cy="2619372"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>112346</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>202223</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>75223</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>154595</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Town">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E945F3E2-4E66-1663-2C22-D1928ADB59BD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Town"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5768731" y="3484685"/>
+              <a:ext cx="1828800" cy="2619372"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331176</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>49824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>40053</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>2196</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Manager">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48090380-1C47-F28F-9DEE-B0A05AD45DF2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Manager"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3867638" y="6204439"/>
+              <a:ext cx="1828800" cy="2619372"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>100622</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>53732</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63499</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>6104</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Category">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D6F0B4A-2353-5D3C-A0C7-E5C4D2A7757B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Category"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5757007" y="6208347"/>
+              <a:ext cx="1828800" cy="2619372"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45391.542820138886" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="13" xr:uid="{103C71B9-F957-C74B-B58D-16E16F7B5E6E}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="salesData"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="Month" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2019-01-01T00:00:00" maxDate="2019-01-02T00:00:00"/>
+    </cacheField>
+    <cacheField name="Store" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Computech"/>
+        <s v="MicroWorld"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Town" numFmtId="0">
+      <sharedItems count="1">
+        <s v="Aberdeen"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Store Code" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Country" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Manager" numFmtId="0">
+      <sharedItems count="11">
+        <s v="Jason Hervey"/>
+        <s v="Spencer Lee"/>
+        <s v="Hugo Matthews"/>
+        <s v="Ben Malone"/>
+        <s v="Kirsty Young"/>
+        <s v="Jade Wilson"/>
+        <s v="Craig Spinks"/>
+        <s v="Nick Fallows"/>
+        <s v="Stephanie Zanoni"/>
+        <s v="Sam Waters"/>
+        <s v="Frank Archibald"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Category" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Mobile Phones"/>
+        <s v="PC's"/>
+        <s v="Laptops"/>
+        <s v="Accessories"/>
+        <s v="Printers"/>
+        <s v="Cameras"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Sales" numFmtId="44">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2064" maxValue="9896" count="13">
+        <n v="9602"/>
+        <n v="6904"/>
+        <n v="9896"/>
+        <n v="5364"/>
+        <n v="7014"/>
+        <n v="5435"/>
+        <n v="4675"/>
+        <n v="7443"/>
+        <n v="7946"/>
+        <n v="3011"/>
+        <n v="6859"/>
+        <n v="2064"/>
+        <n v="4666"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition pivotCacheId="1164331177"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="13">
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="ABD"/>
+    <s v="UK"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="ABD"/>
+    <s v="UK"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="ABD"/>
+    <s v="UK"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="ABD"/>
+    <s v="UK"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="ABD"/>
+    <s v="UK"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="ABD"/>
+    <s v="UK"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="ABD"/>
+    <s v="UK"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="ABD"/>
+    <s v="UK"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="ABD"/>
+    <s v="UK"/>
+    <x v="7"/>
+    <x v="4"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="ABD"/>
+    <s v="UK"/>
+    <x v="8"/>
+    <x v="5"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="ABD"/>
+    <s v="UK"/>
+    <x v="9"/>
+    <x v="5"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="ABD"/>
+    <s v="UK"/>
+    <x v="10"/>
+    <x v="5"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="ABD"/>
+    <s v="UK"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="12"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{29A8BD9E-B2B2-AD4A-B6E7-FBF1629A43D7}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A17:C53" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField numFmtId="14" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0" sortType="descending">
+      <items count="12">
+        <item x="3"/>
+        <item x="6"/>
+        <item x="10"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="7">
+        <item x="3"/>
+        <item x="5"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="44" subtotalTop="0" showAll="0">
+      <items count="14">
+        <item x="11"/>
+        <item x="9"/>
+        <item x="12"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="10"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="5"/>
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="36">
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="default">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i t="default">
+      <x v="6"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Sales" fld="7" baseField="0" baseItem="0" numFmtId="165"/>
+    <dataField name="Average of Sales" fld="7" subtotal="average" baseField="0" baseItem="0" numFmtId="165"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight18" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Store" xr10:uid="{11589D5D-3666-BB4C-B18A-14E49838CB34}" sourceName="Store">
+  <pivotTables>
+    <pivotTable tabId="3" name="PivotTable1"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1164331177">
+      <items count="2">
+        <i x="0" s="1"/>
+        <i x="1" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Town" xr10:uid="{D2741FA5-32C9-544C-B9DA-211D6D177DBE}" sourceName="Town">
+  <pivotTables>
+    <pivotTable tabId="3" name="PivotTable1"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1164331177">
+      <items count="1">
+        <i x="0" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Manager" xr10:uid="{4E2CDF5E-A1FA-534F-A6F6-6E440F0FB4FC}" sourceName="Manager">
+  <pivotTables>
+    <pivotTable tabId="3" name="PivotTable1"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1164331177">
+      <items count="11">
+        <i x="3" s="1"/>
+        <i x="6" s="1"/>
+        <i x="10" s="1"/>
+        <i x="2" s="1"/>
+        <i x="5" s="1"/>
+        <i x="0" s="1"/>
+        <i x="4" s="1"/>
+        <i x="7" s="1"/>
+        <i x="9" s="1"/>
+        <i x="1" s="1"/>
+        <i x="8" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache4.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Category" xr10:uid="{BF550602-C3A7-A245-AD52-7829A3E89E09}" sourceName="Category">
+  <pivotTables>
+    <pivotTable tabId="3" name="PivotTable1"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1164331177">
+      <items count="6">
+        <i x="3" s="1"/>
+        <i x="5" s="1"/>
+        <i x="2" s="1"/>
+        <i x="0" s="1"/>
+        <i x="1" s="1"/>
+        <i x="4" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Store" xr10:uid="{E82BE0BE-D7D4-8147-9A0F-114559333594}" cache="Slicer_Store" caption="Store" style="SlicerStyleLight3" rowHeight="251883"/>
+  <slicer name="Town" xr10:uid="{16065EBE-0059-124F-82A0-7DE0E0A30B1A}" cache="Slicer_Town" caption="Town" style="SlicerStyleLight3" rowHeight="251883"/>
+  <slicer name="Manager" xr10:uid="{9EC8356D-1236-7749-8A4B-5EA38AA90662}" cache="Slicer_Manager" caption="Manager" startItem="4" style="SlicerStyleLight3" rowHeight="251883"/>
+  <slicer name="Category" xr10:uid="{6F169C59-C250-0247-9DA0-06DE7B6FAA48}" cache="Slicer_Category" caption="Category" style="SlicerStyleLight3" rowHeight="251883"/>
+</slicers>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A0B53A20-206D-0042-81BE-367C9FAE2C26}" name="salesData" displayName="salesData" ref="A1:H14" totalsRowShown="0">
+  <autoFilter ref="A1:H14" xr:uid="{A0B53A20-206D-0042-81BE-367C9FAE2C26}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{5B42CC0A-021C-024C-9651-AF48075AFAD3}" name="Month" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{0300BB49-04DA-5C44-A9CB-027323A2E3F5}" name="Store"/>
+    <tableColumn id="3" xr3:uid="{A52A6F7E-4738-4248-B7AF-6821352B1140}" name="Town"/>
+    <tableColumn id="4" xr3:uid="{0096AF72-1489-A446-A7C3-F617AAA4A420}" name="Store Code"/>
+    <tableColumn id="5" xr3:uid="{6ECFD699-B190-734F-A82E-E8763B7BB723}" name="Country"/>
+    <tableColumn id="6" xr3:uid="{F065154F-4DE4-6340-876F-501FE6280AF9}" name="Manager"/>
+    <tableColumn id="7" xr3:uid="{3857855E-A83C-E143-84E8-5231CFBEF054}" name="Category"/>
+    <tableColumn id="8" xr3:uid="{D8BDAAD1-0A23-BF43-8004-F023CB34132A}" name="Sales" dataDxfId="2" dataCellStyle="Currency"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{557D97B2-04F6-354D-B593-FB40EDC12100}" name="Table2" displayName="Table2" ref="A1:E10" totalsRowShown="0">
+  <autoFilter ref="A1:E10" xr:uid="{557D97B2-04F6-354D-B593-FB40EDC12100}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{36372960-A2E8-6047-8249-4040559FEB5E}" name="Category"/>
+    <tableColumn id="2" xr3:uid="{47898722-8262-D043-AAD8-90631F2CA5E3}" name="App"/>
+    <tableColumn id="3" xr3:uid="{C09A75A5-23CF-5E43-9E31-13439D521EB7}" name="Type"/>
+    <tableColumn id="4" xr3:uid="{18B5AB70-7301-2640-B56C-E99BBD54D6C1}" name="Revenue" dataDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{187057D5-EB74-124D-BCFE-866099E14EB4}" name="Profit" dataDxfId="0" dataCellStyle="Currency"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -576,7 +1803,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -907,7 +2134,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -930,11 +2157,11 @@
       <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -1112,14 +2339,1603 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F5989F-007F-9C48-843B-130367F9DFDB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="3">
+        <v>9602</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="3">
+        <v>6904</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="3">
+        <v>9896</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="3">
+        <v>5364</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="3">
+        <v>7014</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="3">
+        <v>5435</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="3">
+        <v>4675</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="3">
+        <v>7443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="3">
+        <v>7946</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="7">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="3">
+        <v>6859</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="3">
+        <v>4666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="H18"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="11">
+        <v>6904</v>
+      </c>
+      <c r="C19" s="11">
+        <v>6904</v>
+      </c>
+      <c r="H19"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="11">
+        <v>7014</v>
+      </c>
+      <c r="C20" s="11">
+        <v>7014</v>
+      </c>
+      <c r="H20"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="11">
+        <v>13918</v>
+      </c>
+      <c r="C21" s="11">
+        <v>6959</v>
+      </c>
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="11">
+        <v>4666</v>
+      </c>
+      <c r="C23" s="11">
+        <v>4666</v>
+      </c>
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="11">
+        <v>7443</v>
+      </c>
+      <c r="C24" s="11">
+        <v>7443</v>
+      </c>
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="11">
+        <v>12109</v>
+      </c>
+      <c r="C25" s="11">
+        <v>6054.5</v>
+      </c>
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="H26"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="11">
+        <v>9896</v>
+      </c>
+      <c r="C27" s="11">
+        <v>9896</v>
+      </c>
+      <c r="H27"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="11">
+        <v>9896</v>
+      </c>
+      <c r="C28" s="11">
+        <v>9896</v>
+      </c>
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="H29"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="11">
+        <v>9602</v>
+      </c>
+      <c r="C30" s="11">
+        <v>9602</v>
+      </c>
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="11">
+        <v>9602</v>
+      </c>
+      <c r="C31" s="11">
+        <v>9602</v>
+      </c>
+      <c r="H31"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="H32"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="11">
+        <v>7946</v>
+      </c>
+      <c r="C33" s="11">
+        <v>7946</v>
+      </c>
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="11">
+        <v>7946</v>
+      </c>
+      <c r="C34" s="11">
+        <v>7946</v>
+      </c>
+      <c r="H34"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="H35"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="11">
+        <v>6859</v>
+      </c>
+      <c r="C36" s="11">
+        <v>6859</v>
+      </c>
+      <c r="H36"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="11">
+        <v>6859</v>
+      </c>
+      <c r="C37" s="11">
+        <v>6859</v>
+      </c>
+      <c r="H37"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="H38"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="11">
+        <v>5435</v>
+      </c>
+      <c r="C39" s="11">
+        <v>5435</v>
+      </c>
+      <c r="H39"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="11">
+        <v>5435</v>
+      </c>
+      <c r="C40" s="11">
+        <v>5435</v>
+      </c>
+      <c r="H40"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="H41"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="11">
+        <v>5364</v>
+      </c>
+      <c r="C42" s="11">
+        <v>5364</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="11">
+        <v>5364</v>
+      </c>
+      <c r="C43" s="11">
+        <v>5364</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="11">
+        <v>4675</v>
+      </c>
+      <c r="C45" s="11">
+        <v>4675</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="11">
+        <v>4675</v>
+      </c>
+      <c r="C46" s="11">
+        <v>4675</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" s="11">
+        <v>3011</v>
+      </c>
+      <c r="C48" s="11">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="11">
+        <v>3011</v>
+      </c>
+      <c r="C49" s="11">
+        <v>3011</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51" s="11">
+        <v>2064</v>
+      </c>
+      <c r="C51" s="11">
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="11">
+        <v>2064</v>
+      </c>
+      <c r="C52" s="11">
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" s="11">
+        <v>80879</v>
+      </c>
+      <c r="C53" s="11">
+        <v>6221.4615384615381</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId4"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F96FF93-2A20-E540-B062-EA8F27FA93C5}">
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="J1" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="N1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="3">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="4"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="str" cm="1">
+        <f t="array" ref="F3:H3">_xlfn._xlws.FILTER($A$2:$C$5, ($A$2:$A$5 = "Apple"), "No records found")</f>
+        <v>Apple</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="J3" t="str" cm="1">
+        <f t="array" ref="J3:L6">_xlfn._xlws.SORT($A$2:$C$5, 2, -1)</f>
+        <v>Apple</v>
+      </c>
+      <c r="K3" s="3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="N3" t="str" cm="1">
+        <f t="array" ref="N3:N6">_xlfn.UNIQUE(A2:A5)</f>
+        <v>Apple</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="F4" t="str" cm="1">
+        <f t="array" ref="F4:H4">_xlfn._xlws.FILTER($A$2:$C$5, ($A$2:$A$5 = "Orange"), "No records found")</f>
+        <v>Orange</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Grapes</v>
+      </c>
+      <c r="K4" s="3">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>12</v>
+      </c>
+      <c r="N4" t="str">
+        <v>Orange</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="13">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12">
+        <v>12</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Orange</v>
+      </c>
+      <c r="K5" s="3">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="N5" t="str">
+        <v>Banana</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="array" ref="C6">SUM(B2:B5*C2:C5)</f>
+        <v>129</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Banana</v>
+      </c>
+      <c r="K6" s="3">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>8</v>
+      </c>
+      <c r="N6" t="str">
+        <v>Grapes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F8" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F9" cm="1">
+        <f t="array" aca="1" ref="F9:H13" ca="1">_xlfn.RANDARRAY(5, 3, 0, 1000, FALSE)</f>
+        <v>531.81049313586311</v>
+      </c>
+      <c r="G9">
+        <f ca="1"/>
+        <v>602.74149481552809</v>
+      </c>
+      <c r="H9">
+        <f ca="1"/>
+        <v>725.19304794926973</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <f ca="1"/>
+        <v>77.470850206571868</v>
+      </c>
+      <c r="G10">
+        <f ca="1"/>
+        <v>760.56468166504555</v>
+      </c>
+      <c r="H10">
+        <f ca="1"/>
+        <v>642.1308045286795</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <f ca="1"/>
+        <v>474.65405752711229</v>
+      </c>
+      <c r="G11">
+        <f ca="1"/>
+        <v>991.59381994791886</v>
+      </c>
+      <c r="H11">
+        <f ca="1"/>
+        <v>278.08867966652338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <f ca="1"/>
+        <v>774.1479507123513</v>
+      </c>
+      <c r="G12">
+        <f ca="1"/>
+        <v>932.67481200160853</v>
+      </c>
+      <c r="H12">
+        <f ca="1"/>
+        <v>923.73780721191633</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <f ca="1"/>
+        <v>90.522831156648635</v>
+      </c>
+      <c r="G13">
+        <f ca="1"/>
+        <v>84.890730087758016</v>
+      </c>
+      <c r="H13">
+        <f ca="1"/>
+        <v>763.10995571771878</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="J1:L1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B82249D9-6F77-0444-99F7-B0A52EB7F2A6}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" cm="1">
+        <f t="array" ref="A1:J10">_xlfn.SEQUENCE(10, 10, 0, 10)</f>
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+      <c r="C1">
+        <v>20</v>
+      </c>
+      <c r="D1">
+        <v>30</v>
+      </c>
+      <c r="E1">
+        <v>40</v>
+      </c>
+      <c r="F1">
+        <v>50</v>
+      </c>
+      <c r="G1">
+        <v>60</v>
+      </c>
+      <c r="H1">
+        <v>70</v>
+      </c>
+      <c r="I1">
+        <v>80</v>
+      </c>
+      <c r="J1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>110</v>
+      </c>
+      <c r="C2">
+        <v>120</v>
+      </c>
+      <c r="D2">
+        <v>130</v>
+      </c>
+      <c r="E2">
+        <v>140</v>
+      </c>
+      <c r="F2">
+        <v>150</v>
+      </c>
+      <c r="G2">
+        <v>160</v>
+      </c>
+      <c r="H2">
+        <v>170</v>
+      </c>
+      <c r="I2">
+        <v>180</v>
+      </c>
+      <c r="J2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>200</v>
+      </c>
+      <c r="B3">
+        <v>210</v>
+      </c>
+      <c r="C3">
+        <v>220</v>
+      </c>
+      <c r="D3">
+        <v>230</v>
+      </c>
+      <c r="E3">
+        <v>240</v>
+      </c>
+      <c r="F3">
+        <v>250</v>
+      </c>
+      <c r="G3">
+        <v>260</v>
+      </c>
+      <c r="H3">
+        <v>270</v>
+      </c>
+      <c r="I3">
+        <v>280</v>
+      </c>
+      <c r="J3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>300</v>
+      </c>
+      <c r="B4">
+        <v>310</v>
+      </c>
+      <c r="C4">
+        <v>320</v>
+      </c>
+      <c r="D4">
+        <v>330</v>
+      </c>
+      <c r="E4">
+        <v>340</v>
+      </c>
+      <c r="F4">
+        <v>350</v>
+      </c>
+      <c r="G4">
+        <v>360</v>
+      </c>
+      <c r="H4">
+        <v>370</v>
+      </c>
+      <c r="I4">
+        <v>380</v>
+      </c>
+      <c r="J4">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>400</v>
+      </c>
+      <c r="B5">
+        <v>410</v>
+      </c>
+      <c r="C5">
+        <v>420</v>
+      </c>
+      <c r="D5">
+        <v>430</v>
+      </c>
+      <c r="E5">
+        <v>440</v>
+      </c>
+      <c r="F5">
+        <v>450</v>
+      </c>
+      <c r="G5">
+        <v>460</v>
+      </c>
+      <c r="H5">
+        <v>470</v>
+      </c>
+      <c r="I5">
+        <v>480</v>
+      </c>
+      <c r="J5">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>500</v>
+      </c>
+      <c r="B6">
+        <v>510</v>
+      </c>
+      <c r="C6">
+        <v>520</v>
+      </c>
+      <c r="D6">
+        <v>530</v>
+      </c>
+      <c r="E6">
+        <v>540</v>
+      </c>
+      <c r="F6">
+        <v>550</v>
+      </c>
+      <c r="G6">
+        <v>560</v>
+      </c>
+      <c r="H6">
+        <v>570</v>
+      </c>
+      <c r="I6">
+        <v>580</v>
+      </c>
+      <c r="J6">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>600</v>
+      </c>
+      <c r="B7">
+        <v>610</v>
+      </c>
+      <c r="C7">
+        <v>620</v>
+      </c>
+      <c r="D7">
+        <v>630</v>
+      </c>
+      <c r="E7">
+        <v>640</v>
+      </c>
+      <c r="F7">
+        <v>650</v>
+      </c>
+      <c r="G7">
+        <v>660</v>
+      </c>
+      <c r="H7">
+        <v>670</v>
+      </c>
+      <c r="I7">
+        <v>680</v>
+      </c>
+      <c r="J7">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>700</v>
+      </c>
+      <c r="B8">
+        <v>710</v>
+      </c>
+      <c r="C8">
+        <v>720</v>
+      </c>
+      <c r="D8">
+        <v>730</v>
+      </c>
+      <c r="E8">
+        <v>740</v>
+      </c>
+      <c r="F8">
+        <v>750</v>
+      </c>
+      <c r="G8">
+        <v>760</v>
+      </c>
+      <c r="H8">
+        <v>770</v>
+      </c>
+      <c r="I8">
+        <v>780</v>
+      </c>
+      <c r="J8">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>800</v>
+      </c>
+      <c r="B9">
+        <v>810</v>
+      </c>
+      <c r="C9">
+        <v>820</v>
+      </c>
+      <c r="D9">
+        <v>830</v>
+      </c>
+      <c r="E9">
+        <v>840</v>
+      </c>
+      <c r="F9">
+        <v>850</v>
+      </c>
+      <c r="G9">
+        <v>860</v>
+      </c>
+      <c r="H9">
+        <v>870</v>
+      </c>
+      <c r="I9">
+        <v>880</v>
+      </c>
+      <c r="J9">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>900</v>
+      </c>
+      <c r="B10">
+        <v>910</v>
+      </c>
+      <c r="C10">
+        <v>920</v>
+      </c>
+      <c r="D10">
+        <v>930</v>
+      </c>
+      <c r="E10">
+        <v>940</v>
+      </c>
+      <c r="F10">
+        <v>950</v>
+      </c>
+      <c r="G10">
+        <v>960</v>
+      </c>
+      <c r="H10">
+        <v>970</v>
+      </c>
+      <c r="I10">
+        <v>980</v>
+      </c>
+      <c r="J10">
+        <v>990</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0763D1-BA65-AD43-A2C7-DA8795C9399B}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3543590</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1417436</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1460004</v>
+      </c>
+      <c r="E3" s="3">
+        <v>584001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1180914</v>
+      </c>
+      <c r="E4" s="3">
+        <v>472365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3315375</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1326150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="3">
+        <v>989735</v>
+      </c>
+      <c r="E6" s="3">
+        <v>395894</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3376162</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1350464.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4704744</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1881897.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3643081</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1457232.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2379523</v>
+      </c>
+      <c r="E10" s="3">
+        <v>951809</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
IFS, two-way lookup, choose random, extract text
</commit_message>
<xml_diff>
--- a/advanced_tutorial.xlsx
+++ b/advanced_tutorial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mymac/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53658A29-0E35-0648-8CCC-8B9F0DA590C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378B5EAB-CED1-324C-95BC-3C913C7131B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{9E1E0ABE-1EFE-9045-A75B-5CB98AFF96A8}"/>
+    <workbookView xWindow="30240" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="10" xr2:uid="{9E1E0ABE-1EFE-9045-A75B-5CB98AFF96A8}"/>
   </bookViews>
   <sheets>
     <sheet name="namedRanges" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,10 @@
     <sheet name="sequence" sheetId="5" r:id="rId5"/>
     <sheet name="xLookup" sheetId="6" r:id="rId6"/>
     <sheet name="xMatch" sheetId="7" r:id="rId7"/>
+    <sheet name="ifs" sheetId="8" r:id="rId8"/>
+    <sheet name="twoWayLookup" sheetId="9" r:id="rId9"/>
+    <sheet name="chooseRandom" sheetId="10" r:id="rId10"/>
+    <sheet name="extractText" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="Customer">namedRanges!$B$2:$B$15</definedName>
@@ -35,15 +39,15 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId9"/>
-        <x14:slicerCache r:id="rId10"/>
-        <x14:slicerCache r:id="rId11"/>
-        <x14:slicerCache r:id="rId12"/>
+        <x14:slicerCache r:id="rId13"/>
+        <x14:slicerCache r:id="rId14"/>
+        <x14:slicerCache r:id="rId15"/>
+        <x14:slicerCache r:id="rId16"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -90,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="181">
   <si>
     <t>Order #</t>
   </si>
@@ -429,6 +433,210 @@
   </si>
   <si>
     <t>Position</t>
+  </si>
+  <si>
+    <t>Instead of nesting several IF functions, we can use IFS for multiple logical conditions</t>
+  </si>
+  <si>
+    <t>Targets</t>
+  </si>
+  <si>
+    <t>Sales &gt;30000 and &lt;45000 = "Good", Sales &gt;=45000 = "Excellent", Sales &lt;30000 = "Review"</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>GoExplore</t>
+  </si>
+  <si>
+    <t>Wanderlust</t>
+  </si>
+  <si>
+    <t>Footsteps</t>
+  </si>
+  <si>
+    <t>Air2Go</t>
+  </si>
+  <si>
+    <t>Sun and Sails</t>
+  </si>
+  <si>
+    <t>Trekker</t>
+  </si>
+  <si>
+    <t>Travelo</t>
+  </si>
+  <si>
+    <t>Flight Shop</t>
+  </si>
+  <si>
+    <t>Want to select a company and month and return the revenue</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Team Assignment</t>
+  </si>
+  <si>
+    <t>Natasha</t>
+  </si>
+  <si>
+    <t>Angelica</t>
+  </si>
+  <si>
+    <t>Dixie</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Lorena</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Jamie</t>
+  </si>
+  <si>
+    <t>Wayne</t>
+  </si>
+  <si>
+    <t>Frances</t>
+  </si>
+  <si>
+    <t>Kayla</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Jody</t>
+  </si>
+  <si>
+    <t>Margie</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Choices</t>
+  </si>
+  <si>
+    <t>Team A</t>
+  </si>
+  <si>
+    <t>Team B</t>
+  </si>
+  <si>
+    <t>Team C</t>
+  </si>
+  <si>
+    <t>Team D</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Bonnie Moss</t>
+  </si>
+  <si>
+    <t>Cody Fletcher</t>
+  </si>
+  <si>
+    <t>Moses Mcguire</t>
+  </si>
+  <si>
+    <t>Kathy Wong</t>
+  </si>
+  <si>
+    <t>Constance Day</t>
+  </si>
+  <si>
+    <t>Cornelius Warner</t>
+  </si>
+  <si>
+    <t>Arthur Valdez</t>
+  </si>
+  <si>
+    <t>Maureen Newton</t>
+  </si>
+  <si>
+    <t>Jennifer Kelly</t>
+  </si>
+  <si>
+    <t>bmoss@gmail.com</t>
+  </si>
+  <si>
+    <t>cody.fletcher@yahoo.com</t>
+  </si>
+  <si>
+    <t>moses@helloworld.com</t>
+  </si>
+  <si>
+    <t>k_wong@hotmail.com</t>
+  </si>
+  <si>
+    <t>constanceday@outlook.com</t>
+  </si>
+  <si>
+    <t>cwarner78@gmail.com</t>
+  </si>
+  <si>
+    <t>valdeza@hotmail.com</t>
+  </si>
+  <si>
+    <t>mnewton@postmaster.com</t>
+  </si>
+  <si>
+    <t>jen_kelly5@yahoo.com</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Domain</t>
   </si>
 </sst>
 </file>
@@ -441,7 +649,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -490,8 +698,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -510,8 +726,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -537,13 +765,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -562,25 +806,38 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="21">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -590,17 +847,227 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="0"/>
+        <color theme="1"/>
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -671,6 +1138,30 @@
           <color theme="1"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1592,14 +2083,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A0B53A20-206D-0042-81BE-367C9FAE2C26}" name="salesData" displayName="salesData" ref="A1:H14" totalsRowShown="0">
   <autoFilter ref="A1:H14" xr:uid="{A0B53A20-206D-0042-81BE-367C9FAE2C26}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5B42CC0A-021C-024C-9651-AF48075AFAD3}" name="Month" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{5B42CC0A-021C-024C-9651-AF48075AFAD3}" name="Month" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{0300BB49-04DA-5C44-A9CB-027323A2E3F5}" name="Store"/>
     <tableColumn id="3" xr3:uid="{A52A6F7E-4738-4248-B7AF-6821352B1140}" name="Town"/>
     <tableColumn id="4" xr3:uid="{0096AF72-1489-A446-A7C3-F617AAA4A420}" name="Store Code"/>
     <tableColumn id="5" xr3:uid="{6ECFD699-B190-734F-A82E-E8763B7BB723}" name="Country"/>
     <tableColumn id="6" xr3:uid="{F065154F-4DE4-6340-876F-501FE6280AF9}" name="Manager"/>
     <tableColumn id="7" xr3:uid="{3857855E-A83C-E143-84E8-5231CFBEF054}" name="Category"/>
-    <tableColumn id="8" xr3:uid="{D8BDAAD1-0A23-BF43-8004-F023CB34132A}" name="Sales" dataDxfId="6" dataCellStyle="Currency"/>
+    <tableColumn id="8" xr3:uid="{D8BDAAD1-0A23-BF43-8004-F023CB34132A}" name="Sales" dataDxfId="19" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1612,19 +2103,52 @@
     <tableColumn id="1" xr3:uid="{36372960-A2E8-6047-8249-4040559FEB5E}" name="Category"/>
     <tableColumn id="2" xr3:uid="{47898722-8262-D043-AAD8-90631F2CA5E3}" name="App"/>
     <tableColumn id="3" xr3:uid="{C09A75A5-23CF-5E43-9E31-13439D521EB7}" name="Type"/>
-    <tableColumn id="4" xr3:uid="{18B5AB70-7301-2640-B56C-E99BBD54D6C1}" name="Revenue" dataDxfId="5" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{187057D5-EB74-124D-BCFE-866099E14EB4}" name="Profit" dataDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{18B5AB70-7301-2640-B56C-E99BBD54D6C1}" name="Revenue" dataDxfId="18" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{187057D5-EB74-124D-BCFE-866099E14EB4}" name="Profit" dataDxfId="17" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AE579DC0-6BB1-6842-AB81-27E87A41105E}" name="Table3" displayName="Table3" ref="A1:B10" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AE579DC0-6BB1-6842-AB81-27E87A41105E}" name="Table3" displayName="Table3" ref="A1:B10" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A1:B10" xr:uid="{AE579DC0-6BB1-6842-AB81-27E87A41105E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D63C0CB3-590C-924E-B190-3ACDB62D078B}" name="App" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{0398086A-15D2-5D4B-8A92-A505948C9FA0}" name="Profit" dataDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{D63C0CB3-590C-924E-B190-3ACDB62D078B}" name="App" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{0398086A-15D2-5D4B-8A92-A505948C9FA0}" name="Profit" dataDxfId="13" dataCellStyle="Currency"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AE6D541A-D4F3-D441-92F4-BD88E0A42274}" name="Table4" displayName="Table4" ref="A1:M9" totalsRowShown="0" dataDxfId="12" dataCellStyle="Currency">
+  <autoFilter ref="A1:M9" xr:uid="{AE6D541A-D4F3-D441-92F4-BD88E0A42274}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{CDD21061-312A-564F-B9EC-90FBFE9B8621}" name="Company"/>
+    <tableColumn id="2" xr3:uid="{008C20F5-AE34-7C47-AE8C-08FA4B29F00A}" name="Jan" dataDxfId="11" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{22C9BA19-5AE6-2248-AE3B-CE834F66C1C8}" name="Feb" dataDxfId="10" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{468D260B-FC7C-2B49-BC83-DA290C101F51}" name="Mar" dataDxfId="9" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{DE0EC43A-2D15-BC4C-9A18-4E0D85E1CBDB}" name="Apr" dataDxfId="8" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{8173D745-EEE8-494D-96C4-925EB52E8A38}" name="May" dataDxfId="7" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{0520075E-5D8D-C249-8BB3-1E3FFDC6C45E}" name="Jun" dataDxfId="6" dataCellStyle="Currency"/>
+    <tableColumn id="8" xr3:uid="{9DD47154-3428-EA48-9ABF-656ABAA76878}" name="Jul" dataDxfId="5" dataCellStyle="Currency"/>
+    <tableColumn id="9" xr3:uid="{2D411244-3145-734B-829D-8186F647FE98}" name="Aug" dataDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="10" xr3:uid="{863956CB-343B-D14E-BF3A-9ACD664424A9}" name="Sep" dataDxfId="3" dataCellStyle="Currency"/>
+    <tableColumn id="11" xr3:uid="{4FFEE2EF-9C88-BF48-9909-964BB08D8F3B}" name="Oct" dataDxfId="2" dataCellStyle="Currency"/>
+    <tableColumn id="12" xr3:uid="{3DDFA2BC-1ADB-184B-992C-2E444FFD838B}" name="Nov" dataDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="13" xr3:uid="{DFD740B3-E483-E740-BC33-BC546D08CEB0}" name="Dec" dataDxfId="0" dataCellStyle="Currency"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{299AC9D8-7395-5B45-A2B3-6A33186E43AC}" name="Table6" displayName="Table6" ref="A1:B10" totalsRowShown="0">
+  <autoFilter ref="A1:B10" xr:uid="{299AC9D8-7395-5B45-A2B3-6A33186E43AC}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{935D0B24-3F7C-2D46-BB05-A036D347540A}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{224C70A3-8F07-D843-A74D-F2DE87AC4150}" name="Email Address" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2276,12 +2800,382 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F2DF26-B5E1-3F45-8ABA-01F220EDCECE}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" t="str">
+        <f ca="1">CHOOSE(RANDBETWEEN(1, 4), $D$2, $D$3, $D$4, $D$5)</f>
+        <v>Team D</v>
+      </c>
+      <c r="D2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B16" ca="1" si="0">CHOOSE(RANDBETWEEN(1, 4), $D$2, $D$3, $D$4, $D$5)</f>
+        <v>Team C</v>
+      </c>
+      <c r="D3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Team A</v>
+      </c>
+      <c r="D4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Team B</v>
+      </c>
+      <c r="D5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Team A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Team A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Team C</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Team C</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Team B</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Team D</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Team C</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Team B</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Team B</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Team B</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Team C</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEECC76-8620-5B46-A274-569F1720BA65}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" t="str">
+        <f>LEFT(Table6[[#This Row],[Email Address]], FIND("@", Table6[[#This Row],[Email Address]]) - 1)</f>
+        <v>bmoss</v>
+      </c>
+      <c r="E2" t="str">
+        <f>RIGHT(Table6[[#This Row],[Email Address]], LEN(Table6[[#This Row],[Email Address]]) - FIND("@", Table6[[#This Row],[Email Address]]))</f>
+        <v>gmail.com</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" t="str">
+        <f>LEFT(Table6[[#This Row],[Email Address]], FIND("@", Table6[[#This Row],[Email Address]]) - 1)</f>
+        <v>cody.fletcher</v>
+      </c>
+      <c r="E3" t="str">
+        <f>RIGHT(Table6[[#This Row],[Email Address]], LEN(Table6[[#This Row],[Email Address]]) - FIND("@", Table6[[#This Row],[Email Address]]))</f>
+        <v>yahoo.com</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="D4" t="str">
+        <f>LEFT(Table6[[#This Row],[Email Address]], FIND("@", Table6[[#This Row],[Email Address]]) - 1)</f>
+        <v>moses</v>
+      </c>
+      <c r="E4" t="str">
+        <f>RIGHT(Table6[[#This Row],[Email Address]], LEN(Table6[[#This Row],[Email Address]]) - FIND("@", Table6[[#This Row],[Email Address]]))</f>
+        <v>helloworld.com</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5" t="str">
+        <f>LEFT(Table6[[#This Row],[Email Address]], FIND("@", Table6[[#This Row],[Email Address]]) - 1)</f>
+        <v>k_wong</v>
+      </c>
+      <c r="E5" t="str">
+        <f>RIGHT(Table6[[#This Row],[Email Address]], LEN(Table6[[#This Row],[Email Address]]) - FIND("@", Table6[[#This Row],[Email Address]]))</f>
+        <v>hotmail.com</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" t="str">
+        <f>LEFT(Table6[[#This Row],[Email Address]], FIND("@", Table6[[#This Row],[Email Address]]) - 1)</f>
+        <v>constanceday</v>
+      </c>
+      <c r="E6" t="str">
+        <f>RIGHT(Table6[[#This Row],[Email Address]], LEN(Table6[[#This Row],[Email Address]]) - FIND("@", Table6[[#This Row],[Email Address]]))</f>
+        <v>outlook.com</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" t="str">
+        <f>LEFT(Table6[[#This Row],[Email Address]], FIND("@", Table6[[#This Row],[Email Address]]) - 1)</f>
+        <v>cwarner78</v>
+      </c>
+      <c r="E7" t="str">
+        <f>RIGHT(Table6[[#This Row],[Email Address]], LEN(Table6[[#This Row],[Email Address]]) - FIND("@", Table6[[#This Row],[Email Address]]))</f>
+        <v>gmail.com</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" t="str">
+        <f>LEFT(Table6[[#This Row],[Email Address]], FIND("@", Table6[[#This Row],[Email Address]]) - 1)</f>
+        <v>valdeza</v>
+      </c>
+      <c r="E8" t="str">
+        <f>RIGHT(Table6[[#This Row],[Email Address]], LEN(Table6[[#This Row],[Email Address]]) - FIND("@", Table6[[#This Row],[Email Address]]))</f>
+        <v>hotmail.com</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" t="str">
+        <f>LEFT(Table6[[#This Row],[Email Address]], FIND("@", Table6[[#This Row],[Email Address]]) - 1)</f>
+        <v>mnewton</v>
+      </c>
+      <c r="E9" t="str">
+        <f>RIGHT(Table6[[#This Row],[Email Address]], LEN(Table6[[#This Row],[Email Address]]) - FIND("@", Table6[[#This Row],[Email Address]]))</f>
+        <v>postmaster.com</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" t="str">
+        <f>LEFT(Table6[[#This Row],[Email Address]], FIND("@", Table6[[#This Row],[Email Address]]) - 1)</f>
+        <v>jen_kelly5</v>
+      </c>
+      <c r="E10" t="str">
+        <f>RIGHT(Table6[[#This Row],[Email Address]], LEN(Table6[[#This Row],[Email Address]]) - FIND("@", Table6[[#This Row],[Email Address]]))</f>
+        <v>yahoo.com</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A0146E18-8D17-C548-A40E-F5AB72804EE7}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{FA211898-0360-6144-9C57-37AE34DD1F88}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{348BFF2B-782B-CE49-80E9-3BA23B2CDD6B}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{A50EAE48-F11D-C54C-8431-2D1FA5258852}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{683D0493-319A-DD41-A8E6-F326A8BA6B20}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{5358CD0A-4E75-E448-AE8D-DCC24D5539B8}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{5A862B2A-D567-1140-B25C-AB976978AF1D}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{A2D9E03F-76A8-CB4F-84B5-A98A744B921F}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{6E308256-FB62-C14E-81B9-EE1085DC2E6B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId10"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3D7B9E-4D33-E549-B27A-9E142D1213B6}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2304,11 +3198,11 @@
       <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -3284,7 +4178,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3311,16 +4205,16 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="J1" s="14" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="J1" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
       <c r="N1" s="1" t="s">
         <v>92</v>
       </c>
@@ -3472,80 +4366,80 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F9" cm="1">
         <f t="array" aca="1" ref="F9:H13" ca="1">_xlfn.RANDARRAY(5, 3, 0, 1000, FALSE)</f>
-        <v>930.3276775304945</v>
+        <v>331.61217989814065</v>
       </c>
       <c r="G9">
         <f ca="1"/>
-        <v>74.118006996852841</v>
+        <v>969.40642831285675</v>
       </c>
       <c r="H9">
         <f ca="1"/>
-        <v>842.86822006445198</v>
+        <v>393.60311679779613</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F10">
         <f ca="1"/>
-        <v>505.56735316808556</v>
+        <v>59.725149337805874</v>
       </c>
       <c r="G10">
         <f ca="1"/>
-        <v>541.47545257698016</v>
+        <v>595.31740509847202</v>
       </c>
       <c r="H10">
         <f ca="1"/>
-        <v>911.39093985120871</v>
+        <v>954.87839067470304</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F11">
         <f ca="1"/>
-        <v>301.7825805006571</v>
+        <v>767.14987953088018</v>
       </c>
       <c r="G11">
         <f ca="1"/>
-        <v>572.78085295325377</v>
+        <v>252.12515984776917</v>
       </c>
       <c r="H11">
         <f ca="1"/>
-        <v>987.2413589665249</v>
+        <v>107.78143053599229</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F12">
         <f ca="1"/>
-        <v>593.46592393626156</v>
+        <v>948.54989209394955</v>
       </c>
       <c r="G12">
         <f ca="1"/>
-        <v>595.33812821762149</v>
+        <v>896.60896940662678</v>
       </c>
       <c r="H12">
         <f ca="1"/>
-        <v>271.11409733849666</v>
+        <v>965.96711243073503</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F13">
         <f ca="1"/>
-        <v>417.98735604242506</v>
+        <v>492.32742639618982</v>
       </c>
       <c r="G13">
         <f ca="1"/>
-        <v>714.84514090898472</v>
+        <v>554.98287892135886</v>
       </c>
       <c r="H13">
         <f ca="1"/>
-        <v>297.72527018635719</v>
+        <v>514.36046413172392</v>
       </c>
     </row>
   </sheetData>
@@ -3563,7 +4457,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3899,7 +4793,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E10"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3927,7 +4821,7 @@
       <c r="E1" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>111</v>
       </c>
       <c r="H1" s="12" t="s">
@@ -3953,7 +4847,7 @@
       <c r="G2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="17" t="str">
+      <c r="H2" s="16" t="str">
         <f>_xlfn.XLOOKUP($H$1, Table2[App], Table2[Category], "Not found", 0)</f>
         <v>Productivity</v>
       </c>
@@ -3977,7 +4871,7 @@
       <c r="G3" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="17" t="str">
+      <c r="H3" s="16" t="str">
         <f>_xlfn.XLOOKUP($H$1, Table2[App], Table2[Type], "Not found", 0)</f>
         <v>Free</v>
       </c>
@@ -4001,7 +4895,7 @@
       <c r="G4" t="s">
         <v>96</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="17">
         <f>_xlfn.XLOOKUP($H$1, Table2[App], Table2[Profit], "Not found", 0)</f>
         <v>1350464.8</v>
       </c>
@@ -4025,7 +4919,7 @@
       <c r="G5" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="17">
         <f>_xlfn.XLOOKUP($H$1, Table2[App], Table2[Revenue], "Not found", 0)</f>
         <v>3376162</v>
       </c>
@@ -4132,8 +5026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465F9BD4-E49F-6445-AD41-74A61F2AF785}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4145,10 +5039,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>96</v>
       </c>
       <c r="D1" s="12" t="s">
@@ -4159,81 +5053,81 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="18">
         <v>1417436</v>
       </c>
       <c r="D2" t="s">
         <v>112</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="16">
         <f>_xlfn.XMATCH($E$1, Table3[App], 0)</f>
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="18">
         <v>584001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <v>472365</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>1326150</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="18">
         <v>395894</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="18">
         <v>1350464.8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="18">
         <v>1881897.6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="18">
         <v>1457232.4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="18">
         <v>951809</v>
       </c>
     </row>
@@ -4248,4 +5142,555 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE63FE7-6B2E-9947-B760-9AFD27359CC4}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B1" s="20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>48737</v>
+      </c>
+      <c r="B3" t="str" cm="1">
+        <f t="array" ref="B3">_xlfn.IFS(AND(A3 &gt; $D$5, A3 &lt; $D$6), "Good", A3 &gt;= $D$6, "Excellent", A3 &lt; $D$5, "Review")</f>
+        <v>Excellent</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>24578</v>
+      </c>
+      <c r="B4" t="str" cm="1">
+        <f t="array" ref="B4">_xlfn.IFS(AND(A4 &gt; $D$5, A4 &lt; $D$6), "Good", A4 &gt;= $D$6, "Excellent", A4 &lt; $D$5, "Review")</f>
+        <v>Review</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>49160</v>
+      </c>
+      <c r="B5" t="str" cm="1">
+        <f t="array" ref="B5">_xlfn.IFS(AND(A5 &gt; $D$5, A5 &lt; $D$6), "Good", A5 &gt;= $D$6, "Excellent", A5 &lt; $D$5, "Review")</f>
+        <v>Excellent</v>
+      </c>
+      <c r="D5" s="5">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>46115</v>
+      </c>
+      <c r="B6" t="str" cm="1">
+        <f t="array" ref="B6">_xlfn.IFS(AND(A6 &gt; $D$5, A6 &lt; $D$6), "Good", A6 &gt;= $D$6, "Excellent", A6 &lt; $D$5, "Review")</f>
+        <v>Excellent</v>
+      </c>
+      <c r="D6">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>27224</v>
+      </c>
+      <c r="B7" t="str" cm="1">
+        <f t="array" ref="B7">_xlfn.IFS(AND(A7 &gt; $D$5, A7 &lt; $D$6), "Good", A7 &gt;= $D$6, "Excellent", A7 &lt; $D$5, "Review")</f>
+        <v>Review</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>35821</v>
+      </c>
+      <c r="B8" t="str" cm="1">
+        <f t="array" ref="B8">_xlfn.IFS(AND(A8 &gt; $D$5, A8 &lt; $D$6), "Good", A8 &gt;= $D$6, "Excellent", A8 &lt; $D$5, "Review")</f>
+        <v>Good</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>45503</v>
+      </c>
+      <c r="B9" t="str" cm="1">
+        <f t="array" ref="B9">_xlfn.IFS(AND(A9 &gt; $D$5, A9 &lt; $D$6), "Good", A9 &gt;= $D$6, "Excellent", A9 &lt; $D$5, "Review")</f>
+        <v>Excellent</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>43783</v>
+      </c>
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10">_xlfn.IFS(AND(A10 &gt; $D$5, A10 &lt; $D$6), "Good", A10 &gt;= $D$6, "Excellent", A10 &lt; $D$5, "Review")</f>
+        <v>Good</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>33770</v>
+      </c>
+      <c r="B11" t="str" cm="1">
+        <f t="array" ref="B11">_xlfn.IFS(AND(A11 &gt; $D$5, A11 &lt; $D$6), "Good", A11 &gt;= $D$6, "Excellent", A11 &lt; $D$5, "Review")</f>
+        <v>Good</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17408E51-213E-CE4A-A544-BB6B9AF4596D}">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="3">
+        <v>49157.871683115824</v>
+      </c>
+      <c r="C2" s="3">
+        <v>96567.958175687483</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45195.431440591652</v>
+      </c>
+      <c r="E2" s="3">
+        <v>75824.994301287676</v>
+      </c>
+      <c r="F2" s="3">
+        <v>94179.479016834332</v>
+      </c>
+      <c r="G2" s="3">
+        <v>36730.274579689372</v>
+      </c>
+      <c r="H2" s="3">
+        <v>19969.345970491486</v>
+      </c>
+      <c r="I2" s="3">
+        <v>97554.247782552353</v>
+      </c>
+      <c r="J2" s="3">
+        <v>19015.277661997214</v>
+      </c>
+      <c r="K2" s="3">
+        <v>44806.817085418734</v>
+      </c>
+      <c r="L2" s="3">
+        <v>19245.888537401712</v>
+      </c>
+      <c r="M2" s="3">
+        <v>90603.47278447701</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="3">
+        <v>58892.070144997429</v>
+      </c>
+      <c r="C3" s="3">
+        <v>61137.454836572113</v>
+      </c>
+      <c r="D3" s="3">
+        <v>68191.05457321534</v>
+      </c>
+      <c r="E3" s="3">
+        <v>80779.605125161514</v>
+      </c>
+      <c r="F3" s="3">
+        <v>43072.049749101963</v>
+      </c>
+      <c r="G3" s="3">
+        <v>12388.402753291666</v>
+      </c>
+      <c r="H3" s="3">
+        <v>74613.228379003238</v>
+      </c>
+      <c r="I3" s="3">
+        <v>85687.029907597622</v>
+      </c>
+      <c r="J3" s="3">
+        <v>63444.217877655537</v>
+      </c>
+      <c r="K3" s="3">
+        <v>21104.4374706464</v>
+      </c>
+      <c r="L3" s="3">
+        <v>92433.669901928384</v>
+      </c>
+      <c r="M3" s="3">
+        <v>26565.567959635286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="3">
+        <v>24042.991766965701</v>
+      </c>
+      <c r="C4" s="3">
+        <v>30701.659989029562</v>
+      </c>
+      <c r="D4" s="3">
+        <v>42289.774443528251</v>
+      </c>
+      <c r="E4" s="3">
+        <v>25610.761817626175</v>
+      </c>
+      <c r="F4" s="3">
+        <v>64319.288487673126</v>
+      </c>
+      <c r="G4" s="3">
+        <v>63280.368087953902</v>
+      </c>
+      <c r="H4" s="3">
+        <v>34732.289974629981</v>
+      </c>
+      <c r="I4" s="3">
+        <v>14101.962071370246</v>
+      </c>
+      <c r="J4" s="3">
+        <v>60521.888214031016</v>
+      </c>
+      <c r="K4" s="3">
+        <v>22948.501836332682</v>
+      </c>
+      <c r="L4" s="3">
+        <v>29829.881574084357</v>
+      </c>
+      <c r="M4" s="3">
+        <v>19967.689484229399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="3">
+        <v>56725.32985227817</v>
+      </c>
+      <c r="C5" s="3">
+        <v>49701.071891590676</v>
+      </c>
+      <c r="D5" s="3">
+        <v>96367.368781046142</v>
+      </c>
+      <c r="E5" s="3">
+        <v>14710.71021499981</v>
+      </c>
+      <c r="F5" s="3">
+        <v>82562.711981324974</v>
+      </c>
+      <c r="G5" s="3">
+        <v>78420.715067312834</v>
+      </c>
+      <c r="H5" s="3">
+        <v>46608.154876509507</v>
+      </c>
+      <c r="I5" s="3">
+        <v>34151.772556236756</v>
+      </c>
+      <c r="J5" s="3">
+        <v>44607.448943108961</v>
+      </c>
+      <c r="K5" s="3">
+        <v>18148.189897827702</v>
+      </c>
+      <c r="L5" s="3">
+        <v>19257.69317071604</v>
+      </c>
+      <c r="M5" s="3">
+        <v>83005.023691911789</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="3">
+        <v>88765.250696603514</v>
+      </c>
+      <c r="C6" s="3">
+        <v>84997.377905214511</v>
+      </c>
+      <c r="D6" s="3">
+        <v>64246.071657233551</v>
+      </c>
+      <c r="E6" s="3">
+        <v>56013.048347930206</v>
+      </c>
+      <c r="F6" s="3">
+        <v>34260.327439668516</v>
+      </c>
+      <c r="G6" s="3">
+        <v>91990.920099353214</v>
+      </c>
+      <c r="H6" s="3">
+        <v>57428.059249769794</v>
+      </c>
+      <c r="I6" s="3">
+        <v>27922.190704100765</v>
+      </c>
+      <c r="J6" s="3">
+        <v>29054.246081932099</v>
+      </c>
+      <c r="K6" s="3">
+        <v>40938.784952370814</v>
+      </c>
+      <c r="L6" s="3">
+        <v>70314.069633102859</v>
+      </c>
+      <c r="M6" s="3">
+        <v>74929.958124257042</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="3">
+        <v>84636.888221192043</v>
+      </c>
+      <c r="C7" s="3">
+        <v>90964.818434319925</v>
+      </c>
+      <c r="D7" s="3">
+        <v>26065.332466936772</v>
+      </c>
+      <c r="E7" s="3">
+        <v>49631.672614991243</v>
+      </c>
+      <c r="F7" s="3">
+        <v>68476.553618511694</v>
+      </c>
+      <c r="G7" s="3">
+        <v>38393.935904531143</v>
+      </c>
+      <c r="H7" s="3">
+        <v>70922.791378175796</v>
+      </c>
+      <c r="I7" s="3">
+        <v>10104.144137844996</v>
+      </c>
+      <c r="J7" s="3">
+        <v>24291.632331033776</v>
+      </c>
+      <c r="K7" s="3">
+        <v>70679.695223037561</v>
+      </c>
+      <c r="L7" s="3">
+        <v>37521.905166038297</v>
+      </c>
+      <c r="M7" s="3">
+        <v>67920.493678441097</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="3">
+        <v>49877.483444842714</v>
+      </c>
+      <c r="C8" s="3">
+        <v>16039.056040455704</v>
+      </c>
+      <c r="D8" s="3">
+        <v>49807.455525383863</v>
+      </c>
+      <c r="E8" s="3">
+        <v>12462.784938915327</v>
+      </c>
+      <c r="F8" s="3">
+        <v>11692.828774032983</v>
+      </c>
+      <c r="G8" s="3">
+        <v>85775.965291947592</v>
+      </c>
+      <c r="H8" s="3">
+        <v>98554.238980466936</v>
+      </c>
+      <c r="I8" s="3">
+        <v>37939.762324427284</v>
+      </c>
+      <c r="J8" s="3">
+        <v>92397.110229774116</v>
+      </c>
+      <c r="K8" s="3">
+        <v>55718.579601751422</v>
+      </c>
+      <c r="L8" s="3">
+        <v>88892.444102865164</v>
+      </c>
+      <c r="M8" s="3">
+        <v>81808.173874420434</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="3">
+        <v>55201.583269074297</v>
+      </c>
+      <c r="C9" s="3">
+        <v>49996.977716298439</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45354.759352917739</v>
+      </c>
+      <c r="E9" s="3">
+        <v>77520.904039416346</v>
+      </c>
+      <c r="F9" s="3">
+        <v>74060.980024295743</v>
+      </c>
+      <c r="G9" s="3">
+        <v>18224.396478515322</v>
+      </c>
+      <c r="H9" s="3">
+        <v>76706.045605868028</v>
+      </c>
+      <c r="I9" s="3">
+        <v>60643.030693980356</v>
+      </c>
+      <c r="J9" s="3">
+        <v>95710.944733838973</v>
+      </c>
+      <c r="K9" s="3">
+        <v>34871.86813951486</v>
+      </c>
+      <c r="L9" s="3">
+        <v>64195.038628074457</v>
+      </c>
+      <c r="M9" s="3">
+        <v>37804.19794009543</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="24">
+        <f>INDEX(Table4[[Jan]:[Dec]], MATCH(B12, Table4[Company], 0), MATCH(B13, Table4[[#Headers],[Jan]:[Dec]], 0))</f>
+        <v>74613.228379003238</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12" xr:uid="{EECD9780-7C0E-344E-9F23-07DC7B1E87C8}">
+      <formula1>$A$2:$A$9</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13" xr:uid="{01515CB7-D881-E441-93D4-523F2ABD019D}">
+      <formula1>$B$1:$M$1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>